<commit_message>
excel column access optimization; sudoers added to user data
</commit_message>
<xml_diff>
--- a/UnixautomationDataGenerator/data.xlsx
+++ b/UnixautomationDataGenerator/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -51,7 +51,13 @@
     <t>Locked</t>
   </si>
   <si>
+    <t>Sudoers</t>
+  </si>
+  <si>
     <t>user1</t>
+  </si>
+  <si>
+    <t>ALL = (ALL) ALL</t>
   </si>
   <si>
     <t>user2</t>
@@ -301,7 +307,9 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -324,11 +332,11 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>666078</v>
+        <v>709143</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -339,19 +347,22 @@
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2:E11" si="3">RANDBETWEEN(100000, 999999)</f>
-        <v>527317</v>
+        <v>286115</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>919753</v>
+        <v>525499</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -362,19 +373,22 @@
       </c>
       <c r="E3" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>721690</v>
+        <v>960012</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>657992</v>
+        <v>932893</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -385,19 +399,22 @@
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>930738</v>
+        <v>573501</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>488073</v>
+        <v>112679</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -408,19 +425,22 @@
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>424968</v>
+        <v>793217</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>631257</v>
+        <v>863523</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -431,19 +451,22 @@
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>988689</v>
+        <v>328856</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>857297</v>
+        <v>137125</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -454,19 +477,22 @@
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>644523</v>
+        <v>120839</v>
       </c>
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>980211</v>
+        <v>285617</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
@@ -477,19 +503,22 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>613318</v>
+        <v>191010</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>801945</v>
+        <v>315938</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>3</v>
@@ -500,19 +529,22 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>939651</v>
+        <v>257754</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>666293</v>
+        <v>836932</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -523,19 +555,22 @@
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>440117</v>
+        <v>220146</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="G10" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>771702</v>
+        <v>534366</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -546,10 +581,13 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>385525</v>
+        <v>870912</v>
       </c>
       <c r="F11" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -587,16 +625,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -623,172 +661,172 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>197487</v>
+        <v>286225</v>
       </c>
       <c r="C2" s="6" t="str">
         <f t="shared" ref="C2:C11" si="2">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>235</v>
+        <v>20</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D11" si="3">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),B2)</f>
-        <v>/home/user1/197487</v>
+        <v>/home/user1/286225</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>578882</v>
+        <v>890301</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>650</v>
+        <v>670</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user2/578882</v>
+        <v>/home/user2/890301</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>853101</v>
+        <v>161986</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user3/853101</v>
+        <v>/home/user3/161986</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>548463</v>
+        <v>774440</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>516</v>
+        <v>473</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user4/548463</v>
+        <v>/home/user4/774440</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>225178</v>
+        <v>550119</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>576</v>
+        <v>236</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user5/225178</v>
+        <v>/home/user5/550119</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>651574</v>
+        <v>684415</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>562</v>
+        <v>204</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user6/651574</v>
+        <v>/home/user6/684415</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>973005</v>
+        <v>704167</v>
       </c>
       <c r="C8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>207</v>
+        <v>11</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user7/973005</v>
+        <v>/home/user7/704167</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>481608</v>
+        <v>908399</v>
       </c>
       <c r="C9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>600</v>
+        <v>30</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user8/481608</v>
+        <v>/home/user8/908399</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>798237</v>
+        <v>150900</v>
       </c>
       <c r="C10" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>324</v>
+        <v>543</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user9/798237</v>
+        <v>/home/user9/150900</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>659288</v>
+        <v>102049</v>
       </c>
       <c r="C11" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>224</v>
+        <v>773</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user10/659288</v>
+        <v>/home/user10/102049</v>
       </c>
     </row>
     <row r="12">
@@ -3780,19 +3818,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3818,183 +3856,183 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="str">
         <f t="shared" ref="B2:C2" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>298783</v>
+        <v>443330</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="1"/>
-        <v>931818</v>
+        <v>121057</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D11" si="3">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>213</v>
+        <v>502</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E11" si="4">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),C2)</f>
-        <v>/home/user1/931818</v>
+        <v>/home/user1/121057</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="str">
         <f t="shared" ref="B3:C3" si="2">RANDBETWEEN(100000, 999999)</f>
-        <v>682064</v>
+        <v>979534</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="2"/>
-        <v>418062</v>
+        <v>965482</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>665</v>
+        <v>736</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user2/418062</v>
+        <v>/home/user2/965482</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:C4" si="5">RANDBETWEEN(100000, 999999)</f>
-        <v>694555</v>
+        <v>243540</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="5"/>
-        <v>732597</v>
+        <v>494953</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>164</v>
+        <v>267</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user3/732597</v>
+        <v>/home/user3/494953</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" ref="B5:C5" si="6">RANDBETWEEN(100000, 999999)</f>
-        <v>768756</v>
+        <v>919243</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="6"/>
-        <v>562847</v>
+        <v>102475</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>414</v>
+        <v>651</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user4/562847</v>
+        <v>/home/user4/102475</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" ref="B6:C6" si="7">RANDBETWEEN(100000, 999999)</f>
-        <v>789710</v>
+        <v>355154</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="7"/>
-        <v>463451</v>
+        <v>319335</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>667</v>
+        <v>611</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user5/463451</v>
+        <v>/home/user5/319335</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" ref="B7:C7" si="8">RANDBETWEEN(100000, 999999)</f>
-        <v>569894</v>
+        <v>898969</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="8"/>
-        <v>410923</v>
+        <v>152053</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>310</v>
+        <v>274</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user6/410923</v>
+        <v>/home/user6/152053</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" ref="B8:C8" si="9">RANDBETWEEN(100000, 999999)</f>
-        <v>439438</v>
+        <v>799057</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="9"/>
-        <v>530435</v>
+        <v>423984</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>265</v>
+        <v>622</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user7/530435</v>
+        <v>/home/user7/423984</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" ref="B9:C9" si="10">RANDBETWEEN(100000, 999999)</f>
-        <v>577967</v>
+        <v>851810</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="10"/>
-        <v>496944</v>
+        <v>407573</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>701</v>
+        <v>643</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user8/496944</v>
+        <v>/home/user8/407573</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" ref="B10:C10" si="11">RANDBETWEEN(100000, 999999)</f>
-        <v>533659</v>
+        <v>322637</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="11"/>
-        <v>565870</v>
+        <v>764078</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="3"/>
@@ -4002,28 +4040,28 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user9/565870</v>
+        <v>/home/user9/764078</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" ref="B11:C11" si="12">RANDBETWEEN(100000, 999999)</f>
-        <v>856135</v>
+        <v>807832</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="12"/>
-        <v>745936</v>
+        <v>836330</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>324</v>
+        <v>755</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user10/745936</v>
+        <v>/home/user10/836330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sudoer script added; register and run script commands added
</commit_message>
<xml_diff>
--- a/UnixautomationDataGenerator/data.xlsx
+++ b/UnixautomationDataGenerator/data.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="Users" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Directories" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="Files" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Scripts" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="GroupNames">Groups!$A$2:$A$3</definedName>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -98,6 +99,9 @@
   <si>
     <t>Content</t>
   </si>
+  <si>
+    <t>add_sudoer.sh</t>
+  </si>
 </sst>
 </file>
 
@@ -106,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -121,6 +125,10 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="4">
@@ -154,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -170,6 +178,9 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -211,6 +222,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -336,7 +351,7 @@
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>709143</v>
+        <v>504740</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -347,7 +362,7 @@
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2:E11" si="3">RANDBETWEEN(100000, 999999)</f>
-        <v>286115</v>
+        <v>233408</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>0</v>
@@ -362,7 +377,7 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>525499</v>
+        <v>541694</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -373,7 +388,7 @@
       </c>
       <c r="E3" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>960012</v>
+        <v>869241</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
@@ -388,7 +403,7 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>932893</v>
+        <v>745033</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>3</v>
@@ -399,7 +414,7 @@
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>573501</v>
+        <v>521760</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>0</v>
@@ -414,7 +429,7 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>112679</v>
+        <v>340405</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
@@ -425,7 +440,7 @@
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>793217</v>
+        <v>285551</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
@@ -440,7 +455,7 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>863523</v>
+        <v>924060</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -451,7 +466,7 @@
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>328856</v>
+        <v>390383</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>0</v>
@@ -466,7 +481,7 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>137125</v>
+        <v>656581</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -477,7 +492,7 @@
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>120839</v>
+        <v>121196</v>
       </c>
       <c r="F7" s="3" t="b">
         <v>0</v>
@@ -492,7 +507,7 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>285617</v>
+        <v>373894</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>2</v>
@@ -503,7 +518,7 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>191010</v>
+        <v>411939</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>0</v>
@@ -518,7 +533,7 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>315938</v>
+        <v>513849</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>3</v>
@@ -529,7 +544,7 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>257754</v>
+        <v>832375</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
@@ -544,7 +559,7 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>836932</v>
+        <v>627179</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
@@ -555,7 +570,7 @@
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>220146</v>
+        <v>559764</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>0</v>
@@ -570,7 +585,7 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>534366</v>
+        <v>881672</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -581,7 +596,7 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>870912</v>
+        <v>210805</v>
       </c>
       <c r="F11" s="3" t="b">
         <v>1</v>
@@ -665,15 +680,15 @@
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>286225</v>
+        <v>168921</v>
       </c>
       <c r="C2" s="6" t="str">
         <f t="shared" ref="C2:C11" si="2">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>20</v>
+        <v>265</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D11" si="3">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),B2)</f>
-        <v>/home/user1/286225</v>
+        <v>/home/user1/168921</v>
       </c>
     </row>
     <row r="3">
@@ -682,15 +697,15 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>890301</v>
+        <v>855725</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>670</v>
+        <v>456</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user2/890301</v>
+        <v>/home/user2/855725</v>
       </c>
     </row>
     <row r="4">
@@ -699,15 +714,15 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>161986</v>
+        <v>553004</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>362</v>
+        <v>406</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user3/161986</v>
+        <v>/home/user3/553004</v>
       </c>
     </row>
     <row r="5">
@@ -716,15 +731,15 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>774440</v>
+        <v>913207</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>473</v>
+        <v>21</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user4/774440</v>
+        <v>/home/user4/913207</v>
       </c>
     </row>
     <row r="6">
@@ -733,15 +748,15 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>550119</v>
+        <v>992921</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user5/550119</v>
+        <v>/home/user5/992921</v>
       </c>
     </row>
     <row r="7">
@@ -750,15 +765,15 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>684415</v>
+        <v>710163</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user6/684415</v>
+        <v>/home/user6/710163</v>
       </c>
     </row>
     <row r="8">
@@ -767,15 +782,15 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>704167</v>
+        <v>414428</v>
       </c>
       <c r="C8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user7/704167</v>
+        <v>/home/user7/414428</v>
       </c>
     </row>
     <row r="9">
@@ -784,15 +799,15 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>908399</v>
+        <v>476929</v>
       </c>
       <c r="C9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user8/908399</v>
+        <v>/home/user8/476929</v>
       </c>
     </row>
     <row r="10">
@@ -801,15 +816,15 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>150900</v>
+        <v>970266</v>
       </c>
       <c r="C10" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>543</v>
+        <v>274</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user9/150900</v>
+        <v>/home/user9/970266</v>
       </c>
     </row>
     <row r="11">
@@ -818,15 +833,15 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>102049</v>
+        <v>621710</v>
       </c>
       <c r="C11" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>773</v>
+        <v>716</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user10/102049</v>
+        <v>/home/user10/621710</v>
       </c>
     </row>
     <row r="12">
@@ -3860,19 +3875,19 @@
       </c>
       <c r="B2" s="4" t="str">
         <f t="shared" ref="B2:C2" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>443330</v>
+        <v>813469</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="1"/>
-        <v>121057</v>
+        <v>656511</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D11" si="3">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>502</v>
+        <v>5</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E11" si="4">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),C2)</f>
-        <v>/home/user1/121057</v>
+        <v>/home/user1/656511</v>
       </c>
     </row>
     <row r="3">
@@ -3881,19 +3896,19 @@
       </c>
       <c r="B3" s="4" t="str">
         <f t="shared" ref="B3:C3" si="2">RANDBETWEEN(100000, 999999)</f>
-        <v>979534</v>
+        <v>194791</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="2"/>
-        <v>965482</v>
+        <v>403688</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>736</v>
+        <v>660</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user2/965482</v>
+        <v>/home/user2/403688</v>
       </c>
     </row>
     <row r="4">
@@ -3902,19 +3917,19 @@
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:C4" si="5">RANDBETWEEN(100000, 999999)</f>
-        <v>243540</v>
+        <v>266807</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="5"/>
-        <v>494953</v>
+        <v>355367</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>267</v>
+        <v>334</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user3/494953</v>
+        <v>/home/user3/355367</v>
       </c>
     </row>
     <row r="5">
@@ -3923,19 +3938,19 @@
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" ref="B5:C5" si="6">RANDBETWEEN(100000, 999999)</f>
-        <v>919243</v>
+        <v>292283</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="6"/>
-        <v>102475</v>
+        <v>657662</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>651</v>
+        <v>325</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user4/102475</v>
+        <v>/home/user4/657662</v>
       </c>
     </row>
     <row r="6">
@@ -3944,19 +3959,19 @@
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" ref="B6:C6" si="7">RANDBETWEEN(100000, 999999)</f>
-        <v>355154</v>
+        <v>111194</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="7"/>
-        <v>319335</v>
+        <v>488952</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>611</v>
+        <v>536</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user5/319335</v>
+        <v>/home/user5/488952</v>
       </c>
     </row>
     <row r="7">
@@ -3965,19 +3980,19 @@
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" ref="B7:C7" si="8">RANDBETWEEN(100000, 999999)</f>
-        <v>898969</v>
+        <v>523783</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="8"/>
-        <v>152053</v>
+        <v>533657</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>274</v>
+        <v>614</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user6/152053</v>
+        <v>/home/user6/533657</v>
       </c>
     </row>
     <row r="8">
@@ -3986,19 +4001,19 @@
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" ref="B8:C8" si="9">RANDBETWEEN(100000, 999999)</f>
-        <v>799057</v>
+        <v>772692</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="9"/>
-        <v>423984</v>
+        <v>591865</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>622</v>
+        <v>731</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user7/423984</v>
+        <v>/home/user7/591865</v>
       </c>
     </row>
     <row r="9">
@@ -4007,19 +4022,19 @@
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" ref="B9:C9" si="10">RANDBETWEEN(100000, 999999)</f>
-        <v>851810</v>
+        <v>341643</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="10"/>
-        <v>407573</v>
+        <v>650279</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>643</v>
+        <v>426</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user8/407573</v>
+        <v>/home/user8/650279</v>
       </c>
     </row>
     <row r="10">
@@ -4028,19 +4043,19 @@
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" ref="B10:C10" si="11">RANDBETWEEN(100000, 999999)</f>
-        <v>322637</v>
+        <v>546294</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="11"/>
-        <v>764078</v>
+        <v>483980</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>771</v>
+        <v>162</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user9/764078</v>
+        <v>/home/user9/483980</v>
       </c>
     </row>
     <row r="11">
@@ -4049,19 +4064,19 @@
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" ref="B11:C11" si="12">RANDBETWEEN(100000, 999999)</f>
-        <v>807832</v>
+        <v>979083</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="12"/>
-        <v>836330</v>
+        <v>501026</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>755</v>
+        <v>60</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user10/836330</v>
+        <v>/home/user10/501026</v>
       </c>
     </row>
   </sheetData>
@@ -4072,4 +4087,54 @@
   </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="A2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
custom scripts are not data anymore; group sudoers processing added;
</commit_message>
<xml_diff>
--- a/UnixautomationDataGenerator/data.xlsx
+++ b/UnixautomationDataGenerator/data.xlsx
@@ -7,7 +7,6 @@
     <sheet state="visible" name="Users" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Directories" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="Files" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="Scripts" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="GroupNames">Groups!$A$2:$A$3</definedName>
@@ -17,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Sudoers</t>
+  </si>
+  <si>
     <t>administrators</t>
+  </si>
+  <si>
+    <t>ALL = (ALL) ALL</t>
   </si>
   <si>
     <t>power_users</t>
@@ -52,13 +57,7 @@
     <t>Locked</t>
   </si>
   <si>
-    <t>Sudoers</t>
-  </si>
-  <si>
     <t>user1</t>
-  </si>
-  <si>
-    <t>ALL = (ALL) ALL</t>
   </si>
   <si>
     <t>user2</t>
@@ -99,9 +98,6 @@
   <si>
     <t>Content</t>
   </si>
-  <si>
-    <t>add_sudoer.sh</t>
-  </si>
 </sst>
 </file>
 
@@ -110,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -125,10 +121,6 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="4">
@@ -162,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -178,9 +170,6 @@
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -222,10 +211,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -237,7 +222,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -265,28 +252,58 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -308,22 +325,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -347,14 +364,14 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>504740</v>
+        <v>654773</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D11" si="2">CONCAT(CONCAT("/home/",A2),"/.ssh/rsa_id")</f>
@@ -362,13 +379,13 @@
       </c>
       <c r="E2" s="4" t="str">
         <f t="shared" ref="E2:E11" si="3">RANDBETWEEN(100000, 999999)</f>
-        <v>233408</v>
+        <v>283541</v>
       </c>
       <c r="F2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -377,10 +394,10 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>541694</v>
+        <v>367416</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="2"/>
@@ -388,13 +405,13 @@
       </c>
       <c r="E3" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>869241</v>
+        <v>435311</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -403,10 +420,10 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>745033</v>
+        <v>878191</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
@@ -414,13 +431,13 @@
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>521760</v>
+        <v>954186</v>
       </c>
       <c r="F4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -429,10 +446,10 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>340405</v>
+        <v>711998</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
@@ -440,13 +457,13 @@
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>285551</v>
+        <v>890970</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -455,10 +472,10 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>924060</v>
+        <v>661025</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
@@ -466,13 +483,13 @@
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>390383</v>
+        <v>873649</v>
       </c>
       <c r="F6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -481,10 +498,10 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>656581</v>
+        <v>985655</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
@@ -492,13 +509,13 @@
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>121196</v>
+        <v>226595</v>
       </c>
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -507,10 +524,10 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>373894</v>
+        <v>325737</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
@@ -518,13 +535,13 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>411939</v>
+        <v>218337</v>
       </c>
       <c r="F8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -533,10 +550,10 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>513849</v>
+        <v>844074</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="2"/>
@@ -544,13 +561,13 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>832375</v>
+        <v>941405</v>
       </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -559,10 +576,10 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>627179</v>
+        <v>984612</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="2"/>
@@ -570,13 +587,13 @@
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>559764</v>
+        <v>869495</v>
       </c>
       <c r="F10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -585,10 +602,10 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>881672</v>
+        <v>470556</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="2"/>
@@ -596,13 +613,13 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>210805</v>
+        <v>256122</v>
       </c>
       <c r="F11" s="3" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -676,19 +693,19 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>168921</v>
+        <v>982987</v>
       </c>
       <c r="C2" s="6" t="str">
         <f t="shared" ref="C2:C11" si="2">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>265</v>
+        <v>601</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D11" si="3">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),B2)</f>
-        <v>/home/user1/168921</v>
+        <v>/home/user1/982987</v>
       </c>
     </row>
     <row r="3">
@@ -697,15 +714,15 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>855725</v>
+        <v>541243</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>456</v>
+        <v>61</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user2/855725</v>
+        <v>/home/user2/541243</v>
       </c>
     </row>
     <row r="4">
@@ -714,15 +731,15 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>553004</v>
+        <v>911954</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>406</v>
+        <v>600</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user3/553004</v>
+        <v>/home/user3/911954</v>
       </c>
     </row>
     <row r="5">
@@ -731,15 +748,15 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>913207</v>
+        <v>605836</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>436</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user4/913207</v>
+        <v>/home/user4/605836</v>
       </c>
     </row>
     <row r="6">
@@ -748,15 +765,15 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>992921</v>
+        <v>547549</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>230</v>
+        <v>753</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user5/992921</v>
+        <v>/home/user5/547549</v>
       </c>
     </row>
     <row r="7">
@@ -765,15 +782,15 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>710163</v>
+        <v>463342</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>165</v>
+        <v>304</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user6/710163</v>
+        <v>/home/user6/463342</v>
       </c>
     </row>
     <row r="8">
@@ -782,15 +799,15 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>414428</v>
+        <v>155736</v>
       </c>
       <c r="C8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user7/414428</v>
+        <v>/home/user7/155736</v>
       </c>
     </row>
     <row r="9">
@@ -799,15 +816,15 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>476929</v>
+        <v>258344</v>
       </c>
       <c r="C9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>112</v>
+        <v>154</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user8/476929</v>
+        <v>/home/user8/258344</v>
       </c>
     </row>
     <row r="10">
@@ -816,15 +833,15 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>970266</v>
+        <v>633165</v>
       </c>
       <c r="C10" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>274</v>
+        <v>173</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user9/970266</v>
+        <v>/home/user9/633165</v>
       </c>
     </row>
     <row r="11">
@@ -833,15 +850,15 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>621710</v>
+        <v>532578</v>
       </c>
       <c r="C11" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>716</v>
+        <v>164</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user10/621710</v>
+        <v>/home/user10/532578</v>
       </c>
     </row>
     <row r="12">
@@ -3871,23 +3888,23 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="str">
         <f t="shared" ref="B2:C2" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>813469</v>
+        <v>255824</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="1"/>
-        <v>656511</v>
+        <v>366280</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D11" si="3">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>5</v>
+        <v>273</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E11" si="4">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),C2)</f>
-        <v>/home/user1/656511</v>
+        <v>/home/user1/366280</v>
       </c>
     </row>
     <row r="3">
@@ -3896,19 +3913,19 @@
       </c>
       <c r="B3" s="4" t="str">
         <f t="shared" ref="B3:C3" si="2">RANDBETWEEN(100000, 999999)</f>
-        <v>194791</v>
+        <v>757988</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="2"/>
-        <v>403688</v>
+        <v>348523</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>660</v>
+        <v>566</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user2/403688</v>
+        <v>/home/user2/348523</v>
       </c>
     </row>
     <row r="4">
@@ -3917,19 +3934,19 @@
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:C4" si="5">RANDBETWEEN(100000, 999999)</f>
-        <v>266807</v>
+        <v>983576</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="5"/>
-        <v>355367</v>
+        <v>845377</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>334</v>
+        <v>534</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user3/355367</v>
+        <v>/home/user3/845377</v>
       </c>
     </row>
     <row r="5">
@@ -3938,19 +3955,19 @@
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" ref="B5:C5" si="6">RANDBETWEEN(100000, 999999)</f>
-        <v>292283</v>
+        <v>432686</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="6"/>
-        <v>657662</v>
+        <v>989589</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>325</v>
+        <v>254</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user4/657662</v>
+        <v>/home/user4/989589</v>
       </c>
     </row>
     <row r="6">
@@ -3959,19 +3976,19 @@
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" ref="B6:C6" si="7">RANDBETWEEN(100000, 999999)</f>
-        <v>111194</v>
+        <v>217699</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="7"/>
-        <v>488952</v>
+        <v>849321</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>536</v>
+        <v>274</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user5/488952</v>
+        <v>/home/user5/849321</v>
       </c>
     </row>
     <row r="7">
@@ -3980,19 +3997,19 @@
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" ref="B7:C7" si="8">RANDBETWEEN(100000, 999999)</f>
-        <v>523783</v>
+        <v>431480</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="8"/>
-        <v>533657</v>
+        <v>911763</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>614</v>
+        <v>140</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user6/533657</v>
+        <v>/home/user6/911763</v>
       </c>
     </row>
     <row r="8">
@@ -4001,19 +4018,19 @@
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" ref="B8:C8" si="9">RANDBETWEEN(100000, 999999)</f>
-        <v>772692</v>
+        <v>163699</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="9"/>
-        <v>591865</v>
+        <v>586253</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>731</v>
+        <v>503</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user7/591865</v>
+        <v>/home/user7/586253</v>
       </c>
     </row>
     <row r="9">
@@ -4022,19 +4039,19 @@
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" ref="B9:C9" si="10">RANDBETWEEN(100000, 999999)</f>
-        <v>341643</v>
+        <v>215048</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="10"/>
-        <v>650279</v>
+        <v>963868</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>426</v>
+        <v>143</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user8/650279</v>
+        <v>/home/user8/963868</v>
       </c>
     </row>
     <row r="10">
@@ -4043,19 +4060,19 @@
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" ref="B10:C10" si="11">RANDBETWEEN(100000, 999999)</f>
-        <v>546294</v>
+        <v>336558</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="11"/>
-        <v>483980</v>
+        <v>993834</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>162</v>
+        <v>377</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user9/483980</v>
+        <v>/home/user9/993834</v>
       </c>
     </row>
     <row r="11">
@@ -4064,19 +4081,19 @@
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" ref="B11:C11" si="12">RANDBETWEEN(100000, 999999)</f>
-        <v>979083</v>
+        <v>899224</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="12"/>
-        <v>501026</v>
+        <v>525305</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>770</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user10/501026</v>
+        <v>/home/user10/525305</v>
       </c>
     </row>
   </sheetData>
@@ -4087,54 +4104,4 @@
   </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ssh pub key copied to authorized_keys
</commit_message>
<xml_diff>
--- a/UnixautomationDataGenerator/data.xlsx
+++ b/UnixautomationDataGenerator/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>SSH Path</t>
+  </si>
+  <si>
+    <t>SSH Authorized Keys</t>
   </si>
   <si>
     <t>SSH Phrase</t>
@@ -321,6 +324,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="4" max="4" width="30.29"/>
+    <col customWidth="1" min="5" max="5" width="39.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -343,9 +347,11 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -367,11 +373,11 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>801811</v>
+        <v>851775</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -381,23 +387,27 @@
         <v>/home/user1/.ssh/rsa_id</v>
       </c>
       <c r="E2" s="4" t="str">
-        <f t="shared" ref="E2:E11" si="3">RANDBETWEEN(100000, 999999)</f>
-        <v>861166</v>
-      </c>
-      <c r="F2" s="3" t="b">
+        <f t="shared" ref="E2:E11" si="3">CONCAT(CONCAT("/home/",A2),"/.ssh/authorized_keys")</f>
+        <v>/home/user1/.ssh/authorized_keys</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f t="shared" ref="F2:F11" si="4">RANDBETWEEN(100000, 999999)</f>
+        <v>926623</v>
+      </c>
+      <c r="G2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>466443</v>
+        <v>545622</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -408,22 +418,26 @@
       </c>
       <c r="E3" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>151445</v>
-      </c>
-      <c r="F3" s="3" t="b">
+        <v>/home/user2/.ssh/authorized_keys</v>
+      </c>
+      <c r="F3" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>976622</v>
+      </c>
+      <c r="G3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>548414</v>
+        <v>734143</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -434,22 +448,26 @@
       </c>
       <c r="E4" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>444188</v>
-      </c>
-      <c r="F4" s="3" t="b">
+        <v>/home/user3/.ssh/authorized_keys</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>947837</v>
+      </c>
+      <c r="G4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>961012</v>
+        <v>973008</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -460,22 +478,26 @@
       </c>
       <c r="E5" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>494019</v>
-      </c>
-      <c r="F5" s="3" t="b">
+        <v>/home/user4/.ssh/authorized_keys</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>168857</v>
+      </c>
+      <c r="G5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>642612</v>
+        <v>953212</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -486,22 +508,26 @@
       </c>
       <c r="E6" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>412262</v>
-      </c>
-      <c r="F6" s="3" t="b">
+        <v>/home/user5/.ssh/authorized_keys</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>909883</v>
+      </c>
+      <c r="G6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>203612</v>
+        <v>805377</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>2</v>
@@ -512,22 +538,26 @@
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>469776</v>
-      </c>
-      <c r="F7" s="3" t="b">
+        <v>/home/user6/.ssh/authorized_keys</v>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>310719</v>
+      </c>
+      <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>629977</v>
+        <v>116345</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
@@ -538,22 +568,26 @@
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>767078</v>
-      </c>
-      <c r="F8" s="3" t="b">
+        <v>/home/user7/.ssh/authorized_keys</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>771323</v>
+      </c>
+      <c r="G8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>822211</v>
+        <v>561742</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -564,22 +598,26 @@
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>512826</v>
-      </c>
-      <c r="F9" s="3" t="b">
+        <v>/home/user8/.ssh/authorized_keys</v>
+      </c>
+      <c r="F9" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>577669</v>
+      </c>
+      <c r="G9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>154392</v>
+        <v>576072</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
@@ -590,22 +628,26 @@
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>234531</v>
-      </c>
-      <c r="F10" s="3" t="b">
+        <v>/home/user9/.ssh/authorized_keys</v>
+      </c>
+      <c r="F10" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>229468</v>
+      </c>
+      <c r="G10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>785815</v>
+        <v>864858</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -616,12 +658,16 @@
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>137466</v>
-      </c>
-      <c r="F11" s="3" t="b">
+        <v>/home/user10/.ssh/authorized_keys</v>
+      </c>
+      <c r="F11" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>576141</v>
+      </c>
+      <c r="G11" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -640,7 +686,7 @@
     <dataValidation type="list" allowBlank="1" sqref="C2:C1000">
       <formula1>Groups!$A$2:$A</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F1000">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G1000">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -660,16 +706,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -696,172 +742,172 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B11" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>167914</v>
+        <v>595397</v>
       </c>
       <c r="C2" s="6" t="str">
         <f t="shared" ref="C2:C11" si="2">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>172</v>
+        <v>306</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D11" si="3">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),B2)</f>
-        <v>/home/user1/167914</v>
+        <v>/home/user1/595397</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="1"/>
-        <v>506268</v>
+        <v>728200</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>315</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user2/506268</v>
+        <v>/home/user2/728200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="1"/>
-        <v>129773</v>
+        <v>798257</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>706</v>
+        <v>746</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user3/129773</v>
+        <v>/home/user3/798257</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
-        <v>527440</v>
+        <v>747158</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>573</v>
+        <v>537</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user4/527440</v>
+        <v>/home/user4/747158</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>705093</v>
+        <v>992180</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>761</v>
+        <v>361</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user5/705093</v>
+        <v>/home/user5/992180</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>264136</v>
+        <v>676485</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>301</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user6/264136</v>
+        <v>/home/user6/676485</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
-        <v>903908</v>
+        <v>726159</v>
       </c>
       <c r="C8" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>321</v>
+        <v>252</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user7/903908</v>
+        <v>/home/user7/726159</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
-        <v>878317</v>
+        <v>896328</v>
       </c>
       <c r="C9" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>234</v>
+        <v>2</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user8/878317</v>
+        <v>/home/user8/896328</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
-        <v>784836</v>
+        <v>394159</v>
       </c>
       <c r="C10" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>440</v>
+        <v>671</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user9/784836</v>
+        <v>/home/user9/394159</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
-        <v>501901</v>
+        <v>825213</v>
       </c>
       <c r="C11" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="3"/>
-        <v>/home/user10/501901</v>
+        <v>/home/user10/825213</v>
       </c>
     </row>
     <row r="12">
@@ -3853,19 +3899,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -3891,212 +3937,212 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="str">
         <f t="shared" ref="B2:C2" si="1">RANDBETWEEN(100000, 999999)</f>
-        <v>374218</v>
+        <v>694843</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" si="1"/>
-        <v>581376</v>
+        <v>378024</v>
       </c>
       <c r="D2" s="6" t="str">
         <f t="shared" ref="D2:D11" si="3">RANDBETWEEN(0, 7) * 100 + RANDBETWEEN(0, 7) * 10 + RANDBETWEEN(0, 7)</f>
-        <v>234</v>
+        <v>743</v>
       </c>
       <c r="E2" t="str">
         <f t="shared" ref="E2:E11" si="4">CONCAT(CONCAT(CONCAT("/home/",A2),"/"),C2)</f>
-        <v>/home/user1/581376</v>
+        <v>/home/user1/378024</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="str">
         <f t="shared" ref="B3:C3" si="2">RANDBETWEEN(100000, 999999)</f>
-        <v>865130</v>
+        <v>287194</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="2"/>
-        <v>286968</v>
+        <v>175642</v>
       </c>
       <c r="D3" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>617</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user2/286968</v>
+        <v>/home/user2/175642</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:C4" si="5">RANDBETWEEN(100000, 999999)</f>
-        <v>506349</v>
+        <v>754229</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="5"/>
-        <v>840493</v>
+        <v>724090</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>777</v>
+        <v>750</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user3/840493</v>
+        <v>/home/user3/724090</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="str">
         <f t="shared" ref="B5:C5" si="6">RANDBETWEEN(100000, 999999)</f>
-        <v>544307</v>
+        <v>869910</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="6"/>
-        <v>586200</v>
+        <v>537304</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>167</v>
+        <v>4</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user4/586200</v>
+        <v>/home/user4/537304</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="str">
         <f t="shared" ref="B6:C6" si="7">RANDBETWEEN(100000, 999999)</f>
-        <v>775927</v>
+        <v>699587</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="7"/>
-        <v>453170</v>
+        <v>394373</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>541</v>
+        <v>570</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user5/453170</v>
+        <v>/home/user5/394373</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="str">
         <f t="shared" ref="B7:C7" si="8">RANDBETWEEN(100000, 999999)</f>
-        <v>293227</v>
+        <v>581811</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="8"/>
-        <v>513136</v>
+        <v>486467</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>672</v>
+        <v>16</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user6/513136</v>
+        <v>/home/user6/486467</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="str">
         <f t="shared" ref="B8:C8" si="9">RANDBETWEEN(100000, 999999)</f>
-        <v>658103</v>
+        <v>182135</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="9"/>
-        <v>252499</v>
+        <v>790163</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>24</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user7/252499</v>
+        <v>/home/user7/790163</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="str">
         <f t="shared" ref="B9:C9" si="10">RANDBETWEEN(100000, 999999)</f>
-        <v>293417</v>
+        <v>820782</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="10"/>
-        <v>979379</v>
+        <v>132803</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user8/979379</v>
+        <v>/home/user8/132803</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4" t="str">
         <f t="shared" ref="B10:C10" si="11">RANDBETWEEN(100000, 999999)</f>
-        <v>955316</v>
+        <v>594264</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="11"/>
-        <v>691208</v>
+        <v>875093</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>662</v>
+        <v>53</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user9/691208</v>
+        <v>/home/user9/875093</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4" t="str">
         <f t="shared" ref="B11:C11" si="12">RANDBETWEEN(100000, 999999)</f>
-        <v>874386</v>
+        <v>969626</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="12"/>
-        <v>313359</v>
+        <v>660816</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>401</v>
+        <v>144</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="4"/>
-        <v>/home/user10/313359</v>
+        <v>/home/user10/660816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>